<commit_message>
Forgot Password dan update login
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -54,9 +54,6 @@
     <t>PasswordEmpty</t>
   </si>
   <si>
-    <t>wrongNpk</t>
-  </si>
-  <si>
     <t>wrongPassword</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>wrongNPK</t>
   </si>
   <si>
-    <t>emptyPasswordComfirm</t>
-  </si>
-  <si>
     <t>emptyNewPassword</t>
   </si>
   <si>
@@ -127,6 +121,21 @@
   </si>
   <si>
     <t>wrongOTP</t>
+  </si>
+  <si>
+    <t>remember</t>
+  </si>
+  <si>
+    <t>emptyPasswordConfirm</t>
+  </si>
+  <si>
+    <t>1a2b3c</t>
+  </si>
+  <si>
+    <t>npkNotFound</t>
+  </si>
+  <si>
+    <t>fail1</t>
   </si>
 </sst>
 </file>
@@ -163,8 +172,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,10 +517,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>55555</v>
+        <v>14426</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -522,13 +534,13 @@
         <v>14426</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -539,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -549,10 +561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,56 +583,56 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>55555</v>
+      <c r="A3" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -631,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -645,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -659,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -670,13 +682,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -684,16 +696,16 @@
         <v>14426</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -701,51 +713,27 @@
         <v>14426</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
         <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>14426</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
-      <c r="I10">
-        <v>9</v>
+        <v>55555</v>
       </c>
       <c r="J10" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -758,8 +746,61 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>14426</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User - Pengaturan Email
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
     <sheet name="User - Forgot Password" sheetId="2" r:id="rId2"/>
+    <sheet name="User - Pengaturan Email" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -136,16 +137,52 @@
   </si>
   <si>
     <t>fail1</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>kondisi</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>emptyEmail</t>
+  </si>
+  <si>
+    <t>yoke</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>dennaleksanti@gmail.com</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>yokebethdenna@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -169,16 +206,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
@@ -806,4 +846,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
User - Ganti Password
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
     <sheet name="User - Forgot Password" sheetId="2" r:id="rId2"/>
     <sheet name="User - Pengaturan Email" sheetId="3" r:id="rId3"/>
+    <sheet name="User - Ganti Password" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -164,6 +165,42 @@
   </si>
   <si>
     <t>yokebethdenna@gmail.com</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>emptyAll</t>
+  </si>
+  <si>
+    <t>Password3</t>
+  </si>
+  <si>
+    <t>emptyCurrentPassword</t>
+  </si>
+  <si>
+    <t>emptyConfirmPassword</t>
+  </si>
+  <si>
+    <t>Password10</t>
+  </si>
+  <si>
+    <t>invalidCurrentPassword</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>invalidNewPassword</t>
+  </si>
+  <si>
+    <t>Password4</t>
+  </si>
+  <si>
+    <t>notMatch</t>
   </si>
 </sst>
 </file>
@@ -852,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -917,4 +954,245 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update forgot and change password (user)
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="71">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -232,7 +232,16 @@
     <t>!@#$%^&amp;*()_</t>
   </si>
   <si>
-    <t>Passwordddddddddddddddddddddddddddddddddddddddddddddddd</t>
+    <t>Passworddddddddddddddddddddddddddddddddddddddddddddddddd2</t>
+  </si>
+  <si>
+    <t>Passworddddddddddddddddddddddddddddddddddddddddddddd</t>
+  </si>
+  <si>
+    <t>Password5</t>
+  </si>
+  <si>
+    <t>Password6</t>
   </si>
 </sst>
 </file>
@@ -686,10 +695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,11 +863,11 @@
       <c r="A10">
         <v>14426</v>
       </c>
-      <c r="B10" s="6">
-        <v>123456</v>
-      </c>
-      <c r="C10" s="6">
-        <v>123456</v>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
       </c>
       <c r="J10" t="s">
         <v>4</v>
@@ -871,11 +880,11 @@
       <c r="A11">
         <v>14426</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
+      <c r="B11" s="6">
+        <v>123456</v>
+      </c>
+      <c r="C11" s="6">
+        <v>123456</v>
       </c>
       <c r="J11" t="s">
         <v>4</v>
@@ -888,11 +897,11 @@
       <c r="A12">
         <v>14426</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
       </c>
       <c r="J12" t="s">
         <v>4</v>
@@ -905,63 +914,45 @@
       <c r="A13">
         <v>14426</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
+      <c r="B13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="J13" t="s">
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>55555</v>
+        <v>14426</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="K14" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14426</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>9</v>
-      </c>
-      <c r="F15">
-        <v>9</v>
-      </c>
-      <c r="G15">
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <v>8</v>
-      </c>
-      <c r="I15">
-        <v>9</v>
+        <v>55555</v>
       </c>
       <c r="J15" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="K15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -975,10 +966,10 @@
         <v>7</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>9</v>
@@ -987,19 +978,54 @@
         <v>9</v>
       </c>
       <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14426</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="I16">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
         <v>1</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B12" r:id="rId1"/>
-    <hyperlink ref="C12" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1078,17 +1104,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="63" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" customWidth="1"/>
     <col min="11" max="11" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1216,103 +1242,192 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
         <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <v>6</v>
+        <v>56</v>
+      </c>
+      <c r="B10" s="6">
+        <v>123456</v>
+      </c>
+      <c r="C10" s="6">
+        <v>123456</v>
       </c>
       <c r="J10" t="s">
         <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="D11">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
         <v>9</v>
       </c>
-      <c r="G11">
+      <c r="G16">
         <v>9</v>
       </c>
-      <c r="H11">
+      <c r="H16">
         <v>2</v>
       </c>
-      <c r="I11">
+      <c r="I16">
         <v>1</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J16" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1"/>
+    <hyperlink ref="C12" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Admin - Manage Test - Pretest and Posttest - Edit
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="User - Ganti Password" sheetId="4" r:id="rId4"/>
     <sheet name="User - Minta Dukungan" sheetId="5" r:id="rId5"/>
     <sheet name="User - FAQ - Search" sheetId="6" r:id="rId6"/>
+    <sheet name="Admin-MT-PrePost- Delete" sheetId="8" r:id="rId7"/>
+    <sheet name="Admin-MT-PrePost- Edit" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -242,6 +244,57 @@
   </si>
   <si>
     <t>Password6</t>
+  </si>
+  <si>
+    <t>searchID</t>
+  </si>
+  <si>
+    <t>serachID</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>tipeSoal</t>
+  </si>
+  <si>
+    <t>jobFunction</t>
+  </si>
+  <si>
+    <t>jobPosition</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>technicalCompetence</t>
+  </si>
+  <si>
+    <t>levelCompetence</t>
+  </si>
+  <si>
+    <t>soal</t>
+  </si>
+  <si>
+    <t>jawabanUraian</t>
+  </si>
+  <si>
+    <t>jawabanBenarSalah</t>
+  </si>
+  <si>
+    <t>jawabanA</t>
+  </si>
+  <si>
+    <t>jawabanB</t>
+  </si>
+  <si>
+    <t>jawabanC</t>
+  </si>
+  <si>
+    <t>jawabanD</t>
+  </si>
+  <si>
+    <t>jawabanABCD</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1527,4 +1580,144 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1771</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1771</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Admin - Manage Test - Pretest and Posttest - Edit (Update)
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="116">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -295,6 +295,90 @@
   </si>
   <si>
     <t>jawabanABCD</t>
+  </si>
+  <si>
+    <t>Pre-Test</t>
+  </si>
+  <si>
+    <t>Uraian</t>
+  </si>
+  <si>
+    <t>ini jawaban</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>SALES HEAD</t>
+  </si>
+  <si>
+    <t>NEOP ARHO</t>
+  </si>
+  <si>
+    <t>technical</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>ini soal</t>
+  </si>
+  <si>
+    <t>Post-Test</t>
+  </si>
+  <si>
+    <t>Pilihan Ganda</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Benar/Salah</t>
+  </si>
+  <si>
+    <t>Benar</t>
+  </si>
+  <si>
+    <t>emptySoalJawabanUraian</t>
+  </si>
+  <si>
+    <t>emptySoalJawabanPilihanGanda</t>
+  </si>
+  <si>
+    <t>Salah</t>
+  </si>
+  <si>
+    <t>emptySoalUraian</t>
+  </si>
+  <si>
+    <t>emptySoalPilihanGanda</t>
+  </si>
+  <si>
+    <t>emptyJawabanUraian</t>
+  </si>
+  <si>
+    <t>emptyJawabanPilihanGanda</t>
+  </si>
+  <si>
+    <t>emptyJawabanBenarSalah</t>
+  </si>
+  <si>
+    <t>emptySoalBenarSalah</t>
+  </si>
+  <si>
+    <t>emptySoalJawabanBenarSalah</t>
   </si>
 </sst>
 </file>
@@ -347,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -361,6 +445,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1643,22 +1730,27 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="11" width="18.44140625" customWidth="1"/>
     <col min="14" max="14" width="10.77734375" customWidth="1"/>
     <col min="15" max="15" width="10.44140625" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -1717,7 +1809,466 @@
         <v>39</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" t="s">
+        <v>100</v>
+      </c>
+      <c r="M10" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O10" t="s">
+        <v>103</v>
+      </c>
+      <c r="P10" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>4</v>
+      </c>
+      <c r="R10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>1764</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - 11 Juni 2020
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hari Sapto\git\LearningManagementWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA366D0-47B5-40E8-8318-2F886435DFDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="119">
   <si>
     <t>NPK_Username</t>
   </si>
@@ -168,9 +169,6 @@
     <t>cancel</t>
   </si>
   <si>
-    <t>yokebethdenna@gmail.com</t>
-  </si>
-  <si>
     <t>currentPassword</t>
   </si>
   <si>
@@ -379,13 +377,25 @@
   </si>
   <si>
     <t>emptySoalJawabanBenarSalah</t>
+  </si>
+  <si>
+    <t>06677</t>
+  </si>
+  <si>
+    <t>#@ccPerfect2o19#</t>
+  </si>
+  <si>
+    <t>#@ccPerfect2o</t>
+  </si>
+  <si>
+    <t>rizkariz20@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +417,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -431,11 +448,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -449,6 +463,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -730,22 +748,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -767,9 +785,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -778,9 +796,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>14426</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -789,12 +807,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>14426</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -803,12 +821,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>14426</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -817,45 +835,46 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14426</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.21875" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="11" width="22.77734375" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -890,7 +909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>36</v>
       </c>
@@ -898,8 +917,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="J3" t="s">
@@ -909,9 +928,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>14426</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
@@ -920,12 +939,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>14426</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
@@ -934,9 +953,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>14426</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -948,9 +967,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14426</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -965,9 +984,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>14426</v>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -982,15 +1001,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>14426</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
         <v>4</v>
@@ -999,15 +1018,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>14426</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J10" t="s">
         <v>4</v>
@@ -1016,14 +1035,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>14426</v>
-      </c>
-      <c r="B11" s="6">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="5">
         <v>123456</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>123456</v>
       </c>
       <c r="J11" t="s">
@@ -1033,15 +1052,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>14426</v>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J12" t="s">
         <v>4</v>
@@ -1050,15 +1069,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>14426</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="J13" t="s">
         <v>4</v>
@@ -1067,9 +1086,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>14426</v>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -1084,8 +1103,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>55555</v>
       </c>
       <c r="J15" t="s">
@@ -1095,15 +1114,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14426</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1130,15 +1149,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>14426</v>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1163,28 +1182,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1195,7 +1215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -1203,7 +1223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1214,8 +1234,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
@@ -1225,9 +1245,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>45</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1235,38 +1255,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" display="yokebethdenna@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="63" customWidth="1"/>
-    <col min="3" max="3" width="58.33203125" customWidth="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>25</v>
@@ -1293,34 +1312,34 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>4</v>
       </c>
       <c r="K2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
@@ -1329,165 +1348,165 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
       <c r="K5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
         <v>54</v>
       </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="B10" s="5">
+        <v>123456</v>
+      </c>
+      <c r="C10" s="5">
+        <v>123456</v>
+      </c>
+      <c r="J10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="6">
-        <v>123456</v>
-      </c>
-      <c r="C10" s="6">
-        <v>123456</v>
-      </c>
-      <c r="J10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
         <v>4</v>
@@ -1496,15 +1515,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -1531,15 +1550,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1565,30 +1584,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B12" r:id="rId1"/>
-    <hyperlink ref="C12" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>58</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
@@ -1597,17 +1616,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1620,46 +1639,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1670,21 +1689,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
@@ -1693,19 +1712,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1771</v>
       </c>
       <c r="B3" t="s">
@@ -1715,8 +1734,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>1771</v>
       </c>
       <c r="B4" t="s">
@@ -1729,78 +1748,78 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="18" max="18" width="27.33203125" customWidth="1"/>
+    <col min="18" max="18" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" t="s">
         <v>38</v>
@@ -1809,462 +1828,462 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1764</v>
       </c>
       <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" t="s">
-        <v>90</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>1764</v>
       </c>
       <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
         <v>97</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>98</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" t="s">
         <v>99</v>
       </c>
-      <c r="E3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" t="s">
-        <v>96</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>100</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>101</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>102</v>
       </c>
-      <c r="O3" t="s">
-        <v>103</v>
-      </c>
       <c r="P3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1764</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" t="s">
         <v>104</v>
-      </c>
-      <c r="D4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" t="s">
-        <v>105</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>1764</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>88</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1764</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>1764</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1764</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>1764</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" t="s">
         <v>89</v>
       </c>
-      <c r="D5" t="s">
+      <c r="Q9" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>1764</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
         <v>91</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
         <v>93</v>
       </c>
-      <c r="Q5" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" t="s">
+        <v>102</v>
+      </c>
+      <c r="P10" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>4</v>
+      </c>
+      <c r="R10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>1764</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1764</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
         <v>88</v>
       </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
         <v>91</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F12" t="s">
         <v>92</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G12" t="s">
         <v>93</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H12" t="s">
         <v>94</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I12" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" t="s">
-        <v>4</v>
-      </c>
-      <c r="R6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="Q12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>1764</v>
       </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
         <v>91</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F13" t="s">
         <v>92</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G13" t="s">
         <v>93</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H13" t="s">
         <v>94</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I13" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" t="s">
-        <v>4</v>
-      </c>
-      <c r="R7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="Q13" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>1764</v>
       </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
         <v>91</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F14" t="s">
         <v>92</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G14" t="s">
         <v>93</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H14" t="s">
         <v>94</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I14" t="s">
         <v>95</v>
       </c>
-      <c r="Q8" t="s">
-        <v>4</v>
-      </c>
-      <c r="R8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>1764</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>4</v>
-      </c>
-      <c r="R9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>1764</v>
-      </c>
-      <c r="B10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" t="s">
-        <v>95</v>
-      </c>
-      <c r="L10" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" t="s">
-        <v>101</v>
-      </c>
-      <c r="N10" t="s">
-        <v>102</v>
-      </c>
-      <c r="O10" t="s">
-        <v>103</v>
-      </c>
-      <c r="P10" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>4</v>
-      </c>
-      <c r="R10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>1764</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" t="s">
-        <v>95</v>
-      </c>
-      <c r="K11" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>4</v>
-      </c>
-      <c r="R11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>1764</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" t="s">
-        <v>95</v>
-      </c>
-      <c r="I12" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>4</v>
-      </c>
-      <c r="R12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>1764</v>
-      </c>
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I13" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>4</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="Q14" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>1764</v>
-      </c>
-      <c r="B14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>4</v>
-      </c>
-      <c r="R14" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Rizka - 15 Juni 2020
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA366D0-47B5-40E8-8318-2F886435DFDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B83120-F1B7-42A0-A6DE-2F2BF058BAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Rizka - 16 Juni 2020
</commit_message>
<xml_diff>
--- a/Data Binding Denna.xlsx
+++ b/Data Binding Denna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143795C3-B2FE-4951-A12A-76FF45382AEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE837ED-3097-4780-A393-8CE84ECDCCF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User-Login" sheetId="1" r:id="rId1"/>
@@ -856,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -1626,7 +1626,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>